<commit_message>
stake, ico contracts linked & compiled successfully
</commit_message>
<xml_diff>
--- a/tropium_ico.xlsx
+++ b/tropium_ico.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\eosio_vigor_contracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\eosio_tropium_contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B07DB7-C928-4D5E-BE5C-BD638E980643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902224CF-BFF6-44BA-A00F-FDBC4F32F444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24ECC0CC-CB28-424B-9F73-E80DD11F83F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24ECC0CC-CB28-424B-9F73-E80DD11F83F1}"/>
   </bookViews>
   <sheets>
     <sheet name="fund" sheetId="1" r:id="rId1"/>
     <sheet name="Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="stake" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>disburse_qty</t>
   </si>
@@ -228,6 +229,57 @@
   <si>
     <t xml:space="preserve">[ { "first": "a", "second": "120.0000 VIGOR" }, { "first": "b", "second": "150.0000 VIGOR" } ]
 </t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>kdsbmnsdvb</t>
+  </si>
+  <si>
+    <t>5000.0000 TRPM</t>
+  </si>
+  <si>
+    <t>lock period</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>[doctor1, doctor2, doctor3]</t>
+  </si>
+  <si>
+    <t>psychiatrist</t>
+  </si>
+  <si>
+    <t>[psych1, psych2, psych3, psych4]</t>
+  </si>
+  <si>
+    <t>stake</t>
+  </si>
+  <si>
+    <t>unstake</t>
+  </si>
+  <si>
+    <t>addadmin(type, name)</t>
+  </si>
+  <si>
+    <t>remadmin(type, name)</t>
+  </si>
+  <si>
+    <t>clradmins(type)</t>
+  </si>
+  <si>
+    <t>setlocktime</t>
+  </si>
+  <si>
+    <t>therapist</t>
   </si>
 </sst>
 </file>
@@ -382,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -416,6 +468,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -424,9 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,10 +1032,10 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="15"/>
       <c r="J22" t="s">
         <v>40</v>
       </c>
@@ -1049,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF3D99F-266B-43A4-BCC9-9488E1A5CE3E}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1067,23 +1120,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="4" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1116,17 +1169,17 @@
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
@@ -1202,17 +1255,17 @@
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
@@ -1278,4 +1331,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8F8D6B-870E-4FA1-B3EE-FADE8008237F}">
+  <dimension ref="B3:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>